<commit_message>
adjusting total system portfolio
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP_IL.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP_IL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96285E47-B167-4EF3-A6D2-9B7F60650844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F49C547-3DF3-4815-A8A9-999F149C3132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="927" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,19 @@
     <definedName name="UtilityPV">Table14[UtilityPV]</definedName>
     <definedName name="UtilityPV_Tech">Table14[UtilityPV]</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -5781,7 +5793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AM7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
@@ -6275,10 +6287,10 @@
         <v>0</v>
       </c>
       <c r="M5" s="19">
-        <v>13.638999999999999</v>
+        <v>10.16</v>
       </c>
       <c r="N5" s="19">
-        <v>3.3</v>
+        <v>2.04</v>
       </c>
       <c r="O5" s="19" t="s">
         <v>122</v>
@@ -6384,10 +6396,10 @@
         <v>0</v>
       </c>
       <c r="M6" s="19">
-        <v>5.6829999999999998</v>
+        <v>7.69</v>
       </c>
       <c r="N6" s="19">
-        <v>4.5</v>
+        <v>1.85</v>
       </c>
       <c r="O6" s="19" t="s">
         <v>122</v>

</xml_diff>